<commit_message>
# Gameboard - Solved issue where multiple sprites would overlap/hide eachother - Sprites are automatically dispersed over the tile (in 2x2, 3x3, 4x4, etc.. layout) - Added double-click option to show contents of tile for added readability
# Gameplay
- Improved multi-unit handling
- All checks should now be multi-unit proof
- Started with multi-unit-move function, unfinished
</commit_message>
<xml_diff>
--- a/www/Settings.xlsx
+++ b/www/Settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spelers" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
   <si>
     <t>A</t>
   </si>
@@ -263,9 +263,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>yearStart</t>
-  </si>
-  <si>
     <t>yearCycle</t>
   </si>
   <si>
@@ -326,10 +323,37 @@
     <t>Oppvervlak van bombardemment. Het aantal vakjes RONDOM het target (bombRadius = 0 =&gt; 1x1 target)</t>
   </si>
   <si>
-    <t>Beeldschermresolutie (horizontaal)</t>
-  </si>
-  <si>
-    <t>Beeldschermresolutie (verticaal)</t>
+    <t>Beeldschermresolutie (horizontaal), 0 = automatische detectie!</t>
+  </si>
+  <si>
+    <t>Beeldschermresolutie (verticaal), 0 = automatische detectie!</t>
+  </si>
+  <si>
+    <t>VRW</t>
+  </si>
+  <si>
+    <t>PLT</t>
+  </si>
+  <si>
+    <t>TNK</t>
+  </si>
+  <si>
+    <t>MNE</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>PAR</t>
+  </si>
+  <si>
+    <t>RAD</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>VEG</t>
   </si>
 </sst>
 </file>
@@ -824,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -881,7 +905,7 @@
         <v>3000</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -901,7 +925,7 @@
         <v>3000</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -921,7 +945,7 @@
         <v>3000</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -942,15 +966,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DA11"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="44" width="6.28515625" customWidth="1"/>
+    <col min="45" max="46" width="3.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:105" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>32</v>
       </c>
@@ -973,7 +1001,7 @@
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
     </row>
-    <row r="2" spans="1:105" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
@@ -1004,737 +1032,579 @@
       <c r="J2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="7" t="s">
+      <c r="K2" s="7" t="str">
+        <f>A5</f>
+        <v>TNK</v>
+      </c>
+      <c r="L2" s="7" t="str">
+        <f>A6</f>
+        <v>PLT</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>A7</f>
+        <v>VRW</v>
+      </c>
+      <c r="N2" s="7" t="str">
+        <f>A8</f>
+        <v>MNE</v>
+      </c>
+      <c r="O2" s="7" t="str">
+        <f>A9</f>
+        <v>VEG</v>
+      </c>
+      <c r="P2" s="7" t="str">
+        <f>A10</f>
+        <v>ANT</v>
+      </c>
+      <c r="Q2" s="7" t="str">
+        <f>A11</f>
+        <v>PAR</v>
+      </c>
+      <c r="R2" s="7" t="str">
+        <f>A11</f>
+        <v>PAR</v>
+      </c>
+      <c r="S2" s="7" t="str">
+        <f>A3</f>
+        <v>RAD</v>
+      </c>
+      <c r="T2" s="7" t="str">
+        <f>A4</f>
+        <v>BOM</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="4">
+        <v>500</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>10</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="6">
+        <v>500</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1200</v>
+      </c>
+      <c r="E5">
+        <v>600</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
         <v>4</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3">
+      <c r="M5">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>1200</v>
-      </c>
-      <c r="E3">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6">
+        <v>150</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.25</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>700</v>
+      </c>
+      <c r="E7">
+        <v>350</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>0.1</v>
+      </c>
+      <c r="L7">
+        <v>0.2</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+      <c r="E8">
+        <v>250</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <v>20</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
         <v>600</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>4</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>10</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
+      <c r="E11" s="5">
         <v>300</v>
       </c>
-      <c r="E4">
-        <v>150</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-      <c r="I4">
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5">
         <v>2</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0.25</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>700</v>
-      </c>
-      <c r="E5">
-        <v>350</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5">
-        <v>8</v>
-      </c>
-      <c r="K5">
-        <v>0.1</v>
-      </c>
-      <c r="L5">
-        <v>0.2</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>500</v>
-      </c>
-      <c r="E6">
-        <v>250</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>20</v>
-      </c>
-      <c r="L6">
-        <v>20</v>
-      </c>
-      <c r="M6">
-        <v>20</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>500</v>
-      </c>
-      <c r="E7">
-        <v>250</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>30</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>200</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <v>10</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>10</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:105" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>600</v>
-      </c>
-      <c r="E9" s="6">
-        <v>300</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
-        <v>2</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="O9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>0</v>
-      </c>
-      <c r="R9" s="6">
-        <v>0</v>
-      </c>
-      <c r="S9" s="6">
-        <v>0</v>
-      </c>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6"/>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="6"/>
-      <c r="AG9" s="6"/>
-      <c r="AH9" s="6"/>
-      <c r="AI9" s="6"/>
-      <c r="AJ9" s="6"/>
-      <c r="AK9" s="6"/>
-      <c r="AL9" s="6"/>
-      <c r="AM9" s="6"/>
-      <c r="AN9" s="6"/>
-      <c r="AO9" s="6"/>
-      <c r="AP9" s="6"/>
-      <c r="AQ9" s="6"/>
-      <c r="AR9" s="6"/>
-      <c r="AS9" s="6"/>
-      <c r="AT9" s="6"/>
-      <c r="AU9" s="6"/>
-      <c r="AV9" s="6"/>
-      <c r="AW9" s="6"/>
-      <c r="AX9" s="6"/>
-      <c r="AY9" s="6"/>
-      <c r="AZ9" s="6"/>
-      <c r="BA9" s="6"/>
-      <c r="BB9" s="6"/>
-      <c r="BC9" s="6"/>
-      <c r="BD9" s="6"/>
-      <c r="BE9" s="6"/>
-      <c r="BF9" s="6"/>
-      <c r="BG9" s="6"/>
-      <c r="BH9" s="6"/>
-      <c r="BI9" s="6"/>
-      <c r="BJ9" s="6"/>
-      <c r="BK9" s="6"/>
-      <c r="BL9" s="6"/>
-      <c r="BM9" s="6"/>
-      <c r="BN9" s="6"/>
-      <c r="BO9" s="6"/>
-      <c r="BP9" s="6"/>
-      <c r="BQ9" s="6"/>
-      <c r="BR9" s="6"/>
-      <c r="BS9" s="6"/>
-      <c r="BT9" s="6"/>
-      <c r="BU9" s="6"/>
-      <c r="BV9" s="6"/>
-      <c r="BW9" s="6"/>
-      <c r="BX9" s="6"/>
-      <c r="BY9" s="6"/>
-      <c r="BZ9" s="6"/>
-      <c r="CA9" s="6"/>
-      <c r="CB9" s="6"/>
-      <c r="CC9" s="6"/>
-      <c r="CD9" s="6"/>
-      <c r="CE9" s="6"/>
-      <c r="CF9" s="6"/>
-      <c r="CG9" s="6"/>
-      <c r="CH9" s="6"/>
-      <c r="CI9" s="6"/>
-      <c r="CJ9" s="6"/>
-      <c r="CK9" s="6"/>
-      <c r="CL9" s="6"/>
-      <c r="CM9" s="6"/>
-      <c r="CN9" s="6"/>
-      <c r="CO9" s="6"/>
-      <c r="CP9" s="6"/>
-      <c r="CQ9" s="6"/>
-      <c r="CR9" s="6"/>
-      <c r="CS9" s="6"/>
-      <c r="CT9" s="6"/>
-      <c r="CU9" s="6"/>
-      <c r="CV9" s="6"/>
-      <c r="CW9" s="6"/>
-      <c r="CX9" s="6"/>
-      <c r="CY9" s="6"/>
-      <c r="CZ9" s="6"/>
-      <c r="DA9" s="6"/>
-    </row>
-    <row r="10" spans="1:105" s="4" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1000</v>
-      </c>
-      <c r="E10" s="5">
-        <v>500</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <v>10</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>0</v>
-      </c>
-      <c r="R10" s="5">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5">
-        <v>0</v>
-      </c>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
-      <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="5"/>
-      <c r="AN10" s="5"/>
-      <c r="AO10" s="5"/>
-      <c r="AP10" s="5"/>
-      <c r="AQ10" s="5"/>
-      <c r="AR10" s="5"/>
-      <c r="AS10" s="5"/>
-      <c r="AT10" s="5"/>
-      <c r="AU10" s="5"/>
-      <c r="AV10" s="5"/>
-      <c r="AW10" s="5"/>
-      <c r="AX10" s="5"/>
-      <c r="AY10" s="5"/>
-      <c r="AZ10" s="5"/>
-      <c r="BA10" s="5"/>
-      <c r="BB10" s="5"/>
-      <c r="BC10" s="5"/>
-      <c r="BD10" s="5"/>
-      <c r="BE10" s="5"/>
-      <c r="BF10" s="5"/>
-      <c r="BG10" s="5"/>
-      <c r="BH10" s="5"/>
-      <c r="BI10" s="5"/>
-      <c r="BJ10" s="5"/>
-      <c r="BK10" s="5"/>
-      <c r="BL10" s="5"/>
-      <c r="BM10" s="5"/>
-      <c r="BN10" s="5"/>
-      <c r="BO10" s="5"/>
-      <c r="BP10" s="5"/>
-      <c r="BQ10" s="5"/>
-      <c r="BR10" s="5"/>
-      <c r="BS10" s="5"/>
-      <c r="BT10" s="5"/>
-      <c r="BU10" s="5"/>
-      <c r="BV10" s="5"/>
-      <c r="BW10" s="5"/>
-      <c r="BX10" s="5"/>
-      <c r="BY10" s="5"/>
-      <c r="BZ10" s="5"/>
-      <c r="CA10" s="5"/>
-      <c r="CB10" s="5"/>
-      <c r="CC10" s="5"/>
-      <c r="CD10" s="5"/>
-      <c r="CE10" s="5"/>
-      <c r="CF10" s="5"/>
-      <c r="CG10" s="5"/>
-      <c r="CH10" s="5"/>
-      <c r="CI10" s="5"/>
-      <c r="CJ10" s="5"/>
-      <c r="CK10" s="5"/>
-      <c r="CL10" s="5"/>
-      <c r="CM10" s="5"/>
-      <c r="CN10" s="5"/>
-      <c r="CO10" s="5"/>
-      <c r="CP10" s="5"/>
-      <c r="CQ10" s="5"/>
-      <c r="CR10" s="5"/>
-      <c r="CS10" s="5"/>
-      <c r="CT10" s="5"/>
-      <c r="CU10" s="5"/>
-      <c r="CV10" s="5"/>
-      <c r="CW10" s="5"/>
-      <c r="CX10" s="5"/>
-      <c r="CY10" s="5"/>
-      <c r="CZ10" s="5"/>
-      <c r="DA10" s="5"/>
-    </row>
-    <row r="11" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1000</v>
-      </c>
-      <c r="E11">
-        <v>500</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:S1"/>
@@ -2147,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2160,7 +2030,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2187,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,7 +2068,7 @@
         <v>1945</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2206,7 +2076,10 @@
         <v>78</v>
       </c>
       <c r="B5">
-        <v>1945</v>
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2214,7 +2087,7 @@
         <v>79</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>500</v>
       </c>
       <c r="C6" t="s">
         <v>93</v>
@@ -2225,7 +2098,7 @@
         <v>80</v>
       </c>
       <c r="B7">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="C7" t="s">
         <v>94</v>
@@ -2236,7 +2109,7 @@
         <v>81</v>
       </c>
       <c r="B8">
-        <v>1500</v>
+        <v>0.3</v>
       </c>
       <c r="C8" t="s">
         <v>95</v>
@@ -2247,7 +2120,7 @@
         <v>82</v>
       </c>
       <c r="B9">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>96</v>
@@ -2258,7 +2131,7 @@
         <v>83</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>97</v>
@@ -2280,21 +2153,10 @@
         <v>85</v>
       </c>
       <c r="B12">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13">
-        <v>900</v>
-      </c>
-      <c r="C13" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Visualizaton - Fixed minor issue with multi-unit drawing - Fixed minor issue with multi-unit selection
# Parsing
- Added automatic detection of individual cities from board
- Added support for multi-unit movements (not fully functional)
</commit_message>
<xml_diff>
--- a/www/Settings.xlsx
+++ b/www/Settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Spelers" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="117">
   <si>
     <t>A</t>
   </si>
@@ -89,9 +89,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>Uitleg</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>P3</t>
   </si>
   <si>
-    <t>Dit bestand bevat alle units in het spel en hun eigenschappen. De meeste eigenschappen spreken voor zich. De laatste kolommen bepalen de *relatieve* aanvalskracht van een unit tegen elke andere unit. Dit kun je lezen als: 1 stuk van unit x kan N stuks van unit y verslaan. Nieuwe units kunnen worden toegevoegd door hiervoor regels toe te voegen. Vervolgens moet er per nieuwe unit ook een kolom worden toegevoegd met de naam van de unit. Hierbij dient van alle units te worden ingevuld wat de relatieve kracht is tegen de nieuwe unit. BELANGRIJK: Unit names 'R' en 'B' mogen niet gebruikt worden, omdat die staan voor speciale units 'Radar' en 'Bombardement'</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -161,60 +155,30 @@
     <t>Tank</t>
   </si>
   <si>
-    <t>spr_Tank</t>
-  </si>
-  <si>
     <t>Peleton</t>
   </si>
   <si>
-    <t>spr_Peleton</t>
-  </si>
-  <si>
     <t>Vrachtwagen</t>
   </si>
   <si>
-    <t>spr_Vrachtwagen</t>
-  </si>
-  <si>
     <t>Mijn</t>
   </si>
   <si>
-    <t>spr_Mijn</t>
-  </si>
-  <si>
     <t>Mijnenveger</t>
   </si>
   <si>
-    <t>spr_Mijnenveger</t>
-  </si>
-  <si>
     <t>Antitank</t>
   </si>
   <si>
-    <t>spr_Antitank</t>
-  </si>
-  <si>
     <t>Paratrooper</t>
   </si>
   <si>
-    <t>spr_Paratrooper</t>
-  </si>
-  <si>
     <t>Radar</t>
   </si>
   <si>
-    <t>spr_Radar</t>
-  </si>
-  <si>
     <t>Bom</t>
   </si>
   <si>
-    <t>spr_Bom</t>
-  </si>
-  <si>
-    <t>Dit bestand bevat de definitie van de spelers. Nieuwe spelers kunnen worden toegevoegd door een nieuwe rij te maken en daar alle eigenschappen in te vullen. Player: interne variabele. Label: de naam van de speler. Gold: startkapitaal. Color: kleurcode, kent een brede definitie ('darkred','gold')</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -354,6 +318,66 @@
   </si>
   <si>
     <t>VEG</t>
+  </si>
+  <si>
+    <t>HRT</t>
+  </si>
+  <si>
+    <t>SPW</t>
+  </si>
+  <si>
+    <t>VOS</t>
+  </si>
+  <si>
+    <t>spr_Radar.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Bom.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Tank.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Peleton.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Vrachtwagen.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Mijn.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Mijnenveger.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Antitank.jpeg</t>
+  </si>
+  <si>
+    <t>spr_Paratrooper.jpeg</t>
+  </si>
+  <si>
+    <t>Dit bestand bevat alle units in het spel en hun eigenschappen. De meeste eigenschappen spreken voor zich. De laatste kolommen bepalen de *relatieve* aanvalskracht van een unit tegen elke andere unit. Dit kun je lezen als: 1 stuk van unit x kan N stuks van unit y verslaan. Nieuwe units kunnen worden toegevoegd door hiervoor regels toe te voegen. Vervolgens moet er per nieuwe unit ook een kolom worden toegevoegd met de naam van de unit. Hierbij dient van alle units te worden ingevuld wat de relatieve kracht is tegen de nieuwe unit. BELANGRIJK: units 1&amp;2 (rij 3&amp;4) zijn speciale units. Deze kunnen hernoemd worden, maar gedragen zich altijd zoals een 'Radar' en 'Bombardement', respectievelijk</t>
+  </si>
+  <si>
+    <t>Dit bestand bevat de omschrijving van de kaart. Het aantal vakjes kan worden aangepast door rijen/kolommen toe te voegen of te verwijderen. Steden worden aangegeven met 'C', water met 'W'. Spelersposities worden weeregeven als P1,P2,P3,P4. De volgorde wordt bepaald door de volgorde in de 'Spelers' tab. TIP: de afbeelding dient puur om het maken van de kaart makkelijker te maken. Deze is dus niet per se nodig om een kaart te maken.</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>BUF</t>
+  </si>
+  <si>
+    <t>Buffels</t>
+  </si>
+  <si>
+    <t>Buffels2018</t>
+  </si>
+  <si>
+    <t>firebrick3</t>
+  </si>
+  <si>
+    <t>Dit bestand bevat de definitie van de spelers. Nieuwe spelers kunnen worden toegevoegd door een nieuwe rij te maken en daar alle eigenschappen in te vullen. Player: interne variabele. Label: de naam van de speler. Gold: startkapitaal. Color: kleurcode, zie afbeelding voor beschikbare kleuren</t>
   </si>
 </sst>
 </file>
@@ -429,9 +453,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -440,6 +461,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -471,8 +495,8 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>59543</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>69068</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -846,112 +870,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
+    <row r="1" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>3000</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>3000</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>3000</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6">
+        <v>3000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -968,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,8 +1023,658 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+    </row>
+    <row r="2" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="6" t="str">
+        <f>A5</f>
+        <v>TNK</v>
+      </c>
+      <c r="L2" s="6" t="str">
+        <f>A6</f>
+        <v>PLT</v>
+      </c>
+      <c r="M2" s="6" t="str">
+        <f>A7</f>
+        <v>VRW</v>
+      </c>
+      <c r="N2" s="6" t="str">
+        <f>A8</f>
+        <v>MNE</v>
+      </c>
+      <c r="O2" s="6" t="str">
+        <f>A9</f>
+        <v>VEG</v>
+      </c>
+      <c r="P2" s="6" t="str">
+        <f>A10</f>
+        <v>ANT</v>
+      </c>
+      <c r="Q2" s="6" t="str">
+        <f>A11</f>
+        <v>PAR</v>
+      </c>
+      <c r="R2" s="6" t="str">
+        <f>A11</f>
+        <v>PAR</v>
+      </c>
+      <c r="S2" s="6" t="str">
+        <f>A3</f>
+        <v>RAD</v>
+      </c>
+      <c r="T2" s="6" t="str">
+        <f>A4</f>
+        <v>BOM</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="3">
+        <v>500</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="5">
+        <v>500</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1200</v>
+      </c>
+      <c r="E5">
+        <v>600</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6">
+        <v>150</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.25</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>700</v>
+      </c>
+      <c r="E7">
+        <v>350</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>0.1</v>
+      </c>
+      <c r="L7">
+        <v>0.2</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+      <c r="E8">
+        <v>250</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <v>20</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9">
+        <v>250</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>10</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>600</v>
+      </c>
+      <c r="E11" s="4">
+        <v>300</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" style="2"/>
+    <col min="2" max="16384" width="4.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1000,638 +1694,14 @@
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
-    </row>
-    <row r="2" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="7" t="str">
-        <f>A5</f>
-        <v>TNK</v>
-      </c>
-      <c r="L2" s="7" t="str">
-        <f>A6</f>
-        <v>PLT</v>
-      </c>
-      <c r="M2" s="7" t="str">
-        <f>A7</f>
-        <v>VRW</v>
-      </c>
-      <c r="N2" s="7" t="str">
-        <f>A8</f>
-        <v>MNE</v>
-      </c>
-      <c r="O2" s="7" t="str">
-        <f>A9</f>
-        <v>VEG</v>
-      </c>
-      <c r="P2" s="7" t="str">
-        <f>A10</f>
-        <v>ANT</v>
-      </c>
-      <c r="Q2" s="7" t="str">
-        <f>A11</f>
-        <v>PAR</v>
-      </c>
-      <c r="R2" s="7" t="str">
-        <f>A11</f>
-        <v>PAR</v>
-      </c>
-      <c r="S2" s="7" t="str">
-        <f>A3</f>
-        <v>RAD</v>
-      </c>
-      <c r="T2" s="7" t="str">
-        <f>A4</f>
-        <v>BOM</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1000</v>
-      </c>
-      <c r="E3" s="4">
-        <v>500</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>10</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>0</v>
-      </c>
-      <c r="R3" s="4">
-        <v>0</v>
-      </c>
-      <c r="S3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1000</v>
-      </c>
-      <c r="E4" s="6">
-        <v>500</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>10</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>1200</v>
-      </c>
-      <c r="E5">
-        <v>600</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>10</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>300</v>
-      </c>
-      <c r="E6">
-        <v>150</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0.25</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>700</v>
-      </c>
-      <c r="E7">
-        <v>350</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-      <c r="K7">
-        <v>0.1</v>
-      </c>
-      <c r="L7">
-        <v>0.2</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>500</v>
-      </c>
-      <c r="E8">
-        <v>250</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>10</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>20</v>
-      </c>
-      <c r="L8">
-        <v>20</v>
-      </c>
-      <c r="M8">
-        <v>20</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>500</v>
-      </c>
-      <c r="E9">
-        <v>250</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>30</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>200</v>
-      </c>
-      <c r="E10">
-        <v>100</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>10</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>10</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>10</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>600</v>
-      </c>
-      <c r="E11" s="5">
-        <v>300</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5">
-        <v>2</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-      <c r="N11" s="5">
-        <v>0</v>
-      </c>
-      <c r="O11" s="5">
-        <v>0</v>
-      </c>
-      <c r="P11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>0</v>
-      </c>
-      <c r="R11" s="5">
-        <v>0</v>
-      </c>
-      <c r="S11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA19"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.28515625" style="2"/>
-    <col min="2" max="16384" width="4.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1695,22 +1765,22 @@
         <v>19</v>
       </c>
       <c r="V2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1723,10 +1793,10 @@
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1734,19 +1804,28 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1754,48 +1833,66 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="Q7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1803,22 +1900,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1826,13 +1923,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1840,28 +1937,28 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,22 +1966,22 @@
         <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1892,7 +1989,7 @@
         <v>10</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1900,22 +1997,22 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1923,22 +2020,22 @@
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1946,22 +2043,22 @@
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1969,16 +2066,16 @@
         <v>14</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1986,16 +2083,16 @@
         <v>15</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2009,6 +2106,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AA1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2020,7 +2120,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,134 +2129,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
+      <c r="A1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>1945</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B6">
         <v>500</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <v>1500</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B8">
         <v>0.3</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Feedback reports - improved scaling/breaking for printing - Changed layout/style of some reports - 'empty' parts or a report are now auto-omitted
# Playability
- Fixed bug where wrong unit-names could brake the game
- Fixed but where bomb/radar could not be renamed (hard-coded references)

# Refactoring
- Improved layout of functions in the files
- Added/improved comments
</commit_message>
<xml_diff>
--- a/www/Settings.xlsx
+++ b/www/Settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="9060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Spelers" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="119">
   <si>
     <t>A</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>Dit bestand bevat de definitie van de spelers. Nieuwe spelers kunnen worden toegevoegd door een nieuwe rij te maken en daar alle eigenschappen in te vullen. Player: interne variabele. Label: de naam van de speler. Gold: startkapitaal. Color: kleurcode, zie afbeelding voor beschikbare kleuren</t>
+  </si>
+  <si>
+    <t>maxReportWidth</t>
+  </si>
+  <si>
+    <t>Maximale breedte van rapporten (in karakters). Nuttig voor bijv. uitprinten op bonnen vs a4</t>
   </si>
 </sst>
 </file>
@@ -872,7 +878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1013,7 +1019,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,8 +1668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1809,15 +1815,6 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="Q5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1838,15 +1835,6 @@
       <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="Q6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1867,15 +1855,6 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="Q7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2082,6 +2061,15 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="K17" s="1" t="s">
         <v>26</v>
       </c>
@@ -2098,6 +2086,9 @@
     <row r="18" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2117,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,6 +2250,17 @@
         <v>87</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
# Visuals - Added some custom css to show player color in tabs - fixed bug where action-feedback was sometimes not shown/overwritten
</commit_message>
<xml_diff>
--- a/www/Settings.xlsx
+++ b/www/Settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="9060" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="9060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Spelers" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="119">
   <si>
     <t>A</t>
   </si>
@@ -421,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -447,11 +447,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,6 +497,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -506,7 +543,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -554,7 +597,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -879,22 +928,30 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:XFD1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -1016,42 +1073,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="44" width="6.28515625" customWidth="1"/>
-    <col min="45" max="46" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="43" width="6.28515625" customWidth="1"/>
+    <col min="44" max="45" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:19" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-    </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>31</v>
       </c>
@@ -1079,7 +1152,7 @@
       <c r="I2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="9" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="6" t="str">
@@ -1106,24 +1179,20 @@
         <f>A10</f>
         <v>ANT</v>
       </c>
-      <c r="Q2" s="6" t="str">
+      <c r="Q2" s="9" t="str">
         <f>A11</f>
         <v>PAR</v>
       </c>
       <c r="R2" s="6" t="str">
-        <f>A11</f>
-        <v>PAR</v>
-      </c>
-      <c r="S2" s="6" t="str">
         <f>A3</f>
         <v>RAD</v>
       </c>
-      <c r="T2" s="6" t="str">
+      <c r="S2" s="6" t="str">
         <f>A4</f>
         <v>BOM</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
@@ -1151,7 +1220,7 @@
       <c r="I3" s="3">
         <v>10</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="10">
         <v>0</v>
       </c>
       <c r="K3" s="3">
@@ -1172,7 +1241,7 @@
       <c r="P3" s="3">
         <v>0</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="10">
         <v>0</v>
       </c>
       <c r="R3" s="3">
@@ -1182,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>95</v>
       </c>
@@ -1210,38 +1279,38 @@
       <c r="I4" s="5">
         <v>10</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="11">
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M4" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N4" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O4" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>100</v>
       </c>
       <c r="R4" s="5">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -1269,7 +1338,7 @@
       <c r="I5">
         <v>8</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="12">
         <v>0</v>
       </c>
       <c r="K5">
@@ -1288,10 +1357,10 @@
         <v>10</v>
       </c>
       <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>3</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -1300,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1328,7 +1397,7 @@
       <c r="I6">
         <v>2</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="12">
         <v>0</v>
       </c>
       <c r="K6">
@@ -1347,10 +1416,10 @@
         <v>3</v>
       </c>
       <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>0.5</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1359,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -1387,14 +1456,14 @@
       <c r="I7">
         <v>10</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="12">
         <v>8</v>
       </c>
       <c r="K7">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="L7">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -1406,10 +1475,10 @@
         <v>1</v>
       </c>
       <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>0.5</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1418,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1446,7 +1515,7 @@
       <c r="I8">
         <v>10</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="12">
         <v>0</v>
       </c>
       <c r="K8">
@@ -1459,16 +1528,16 @@
         <v>20</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>20</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1477,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -1505,14 +1574,14 @@
       <c r="I9">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="12">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1524,10 +1593,10 @@
         <v>1</v>
       </c>
       <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>0.25</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1536,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>92</v>
       </c>
@@ -1547,10 +1616,10 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1564,14 +1633,14 @@
       <c r="I10">
         <v>2</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="12">
         <v>0</v>
       </c>
       <c r="K10">
         <v>10</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M10">
         <v>10</v>
@@ -1585,8 +1654,8 @@
       <c r="P10">
         <v>1</v>
       </c>
-      <c r="Q10">
-        <v>1</v>
+      <c r="Q10" s="12">
+        <v>0.5</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -1595,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>93</v>
       </c>
@@ -1603,13 +1672,13 @@
         <v>47</v>
       </c>
       <c r="C11" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="E11" s="4">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1623,44 +1692,44 @@
       <c r="I11" s="4">
         <v>2</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="12">
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="L11" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11" s="4">
         <v>0</v>
       </c>
       <c r="O11" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P11" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="12">
+        <v>1</v>
       </c>
       <c r="R11" s="4">
         <v>0</v>
       </c>
-      <c r="S11" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="S11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1668,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1679,35 +1748,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1815,6 +1884,15 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="Q5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1835,6 +1913,15 @@
       <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1855,6 +1942,15 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="Q7" s="1" t="s">
         <v>29</v>
       </c>
@@ -2061,15 +2157,6 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="K17" s="1" t="s">
         <v>26</v>
       </c>
@@ -2086,9 +2173,6 @@
     <row r="18" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2110,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,14 +2204,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2255,7 +2339,7 @@
         <v>117</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>118</v>

</xml_diff>